<commit_message>
Added additional analysis in spreadsheet functions
</commit_message>
<xml_diff>
--- a/testing/data/Buildings.xlsx
+++ b/testing/data/Buildings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="339">
   <si>
     <t>Site ID</t>
   </si>
@@ -1461,7 +1461,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1471,8 +1471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F103" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L149" sqref="L149"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2486,9 +2486,6 @@
       <c r="G43" t="s">
         <v>331</v>
       </c>
-      <c r="H43" t="s">
-        <v>12</v>
-      </c>
       <c r="I43" t="s">
         <v>12</v>
       </c>

</xml_diff>